<commit_message>
Add Bearing Mount G-Code files
</commit_message>
<xml_diff>
--- a/BOMs/Conveyor/BOM.xlsx
+++ b/BOMs/Conveyor/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Waller\Documents\GitHub\Final-Year-Project\BOMs\Conveyor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF257BD8-0B2B-4D04-838D-F3F359828757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5B96C2-7580-4D79-97D3-E9E29E38BA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-2190" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update STL and BOMs
</commit_message>
<xml_diff>
--- a/BOMs/Conveyor/BOM.xlsx
+++ b/BOMs/Conveyor/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Waller\Documents\GitHub\Final-Year-Project\BOMs\Conveyor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5B96C2-7580-4D79-97D3-E9E29E38BA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAAB84B-2571-417A-BEC1-2BE13CBD381A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2190" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1298,7 @@
       <c r="H7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
       <c r="H9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2084,6 +2084,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I8" r:id="rId1" xr:uid="{C3CF939D-301A-43F9-A972-AC5D060493F4}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{79368489-227A-4287-95BB-26C9ADC125A5}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{34BFDAA4-BAF9-46B2-9772-D943A6BFF576}"/>
+    <hyperlink ref="I9" r:id="rId4" xr:uid="{4DC02E85-CAC8-4CAF-9540-05C6F3CCD1A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>